<commit_message>
Inserts das tabelas para testes
</commit_message>
<xml_diff>
--- a/java/extracao-dados/src/main/java/school/sptech/apachePOI/arquivos/curated-entrada-passageiros-por-linha-2020-2024.xlsx
+++ b/java/extracao-dados/src/main/java/school/sptech/apachePOI/arquivos/curated-entrada-passageiros-por-linha-2020-2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java\Vivi\FluxoCerto\java\conexao-banco\src\main\java\school\sptech\apachePOI\arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\faculdade\FluxoCerto\java\extracao-dados\src\main\java\school\sptech\apachePOI\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342570A0-DAE3-4FCD-94BE-1145ABF9DA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E3B5A5-54D2-4F06-B0D1-B58417EFEEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="69">
   <si>
     <t>Data</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>2020-12-01</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -567,18 +570,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -594,8 +598,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -611,8 +618,11 @@
       <c r="E2">
         <v>759</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -628,8 +638,11 @@
       <c r="E3">
         <v>495</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -645,8 +658,11 @@
       <c r="E4">
         <v>890</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -662,8 +678,11 @@
       <c r="E5">
         <v>829</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -679,8 +698,11 @@
       <c r="E6">
         <v>548</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -696,8 +718,11 @@
       <c r="E7">
         <v>908</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -713,8 +738,11 @@
       <c r="E8">
         <v>852</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -730,8 +758,11 @@
       <c r="E9">
         <v>558</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -747,8 +778,11 @@
       <c r="E10">
         <v>936</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -764,8 +798,11 @@
       <c r="E11">
         <v>844</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -781,8 +818,11 @@
       <c r="E12">
         <v>557</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -798,8 +838,11 @@
       <c r="E13">
         <v>923</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -815,8 +858,11 @@
       <c r="E14">
         <v>844</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -832,8 +878,11 @@
       <c r="E15">
         <v>557</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -849,8 +898,11 @@
       <c r="E16">
         <v>917</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -866,8 +918,11 @@
       <c r="E17">
         <v>848</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -883,8 +938,11 @@
       <c r="E18">
         <v>547</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -900,8 +958,11 @@
       <c r="E19">
         <v>919</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -917,8 +978,11 @@
       <c r="E20">
         <v>774</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -934,8 +998,11 @@
       <c r="E21">
         <v>515</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -951,8 +1018,11 @@
       <c r="E22">
         <v>861</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -968,8 +1038,11 @@
       <c r="E23">
         <v>858</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -985,8 +1058,11 @@
       <c r="E24">
         <v>558</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>15</v>
       </c>
@@ -1002,8 +1078,11 @@
       <c r="E25">
         <v>928</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -1019,8 +1098,11 @@
       <c r="E26">
         <v>874</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
@@ -1036,8 +1118,11 @@
       <c r="E27">
         <v>561</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1053,8 +1138,11 @@
       <c r="E28">
         <v>954</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -1070,8 +1158,11 @@
       <c r="E29">
         <v>869</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -1087,8 +1178,11 @@
       <c r="E30">
         <v>567</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -1104,8 +1198,11 @@
       <c r="E31">
         <v>926</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
@@ -1121,8 +1218,11 @@
       <c r="E32">
         <v>879</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -1138,8 +1238,11 @@
       <c r="E33">
         <v>575</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1155,8 +1258,11 @@
       <c r="E34">
         <v>945</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1172,8 +1278,11 @@
       <c r="E35">
         <v>888</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -1189,8 +1298,11 @@
       <c r="E36">
         <v>566</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -1206,8 +1318,11 @@
       <c r="E37">
         <v>960</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
@@ -1223,8 +1338,11 @@
       <c r="E38">
         <v>725</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
@@ -1240,8 +1358,11 @@
       <c r="E39">
         <v>446</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
@@ -1257,8 +1378,11 @@
       <c r="E40">
         <v>817</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -1274,8 +1398,11 @@
       <c r="E41">
         <v>792</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
@@ -1291,8 +1418,11 @@
       <c r="E42">
         <v>490</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>21</v>
       </c>
@@ -1308,8 +1438,11 @@
       <c r="E43">
         <v>888</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
@@ -1325,8 +1458,11 @@
       <c r="E44">
         <v>828</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
@@ -1342,8 +1478,11 @@
       <c r="E45">
         <v>520</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>22</v>
       </c>
@@ -1359,8 +1498,11 @@
       <c r="E46">
         <v>914</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -1376,8 +1518,11 @@
       <c r="E47">
         <v>830</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
@@ -1393,8 +1538,11 @@
       <c r="E48">
         <v>512</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
@@ -1410,8 +1558,11 @@
       <c r="E49">
         <v>973</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>24</v>
       </c>
@@ -1427,8 +1578,11 @@
       <c r="E50">
         <v>829</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>24</v>
       </c>
@@ -1444,8 +1598,11 @@
       <c r="E51">
         <v>512</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>24</v>
       </c>
@@ -1461,8 +1618,11 @@
       <c r="E52">
         <v>901</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>25</v>
       </c>
@@ -1478,8 +1638,11 @@
       <c r="E53">
         <v>858</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>25</v>
       </c>
@@ -1495,8 +1658,11 @@
       <c r="E54">
         <v>521</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -1512,8 +1678,11 @@
       <c r="E55">
         <v>932</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>26</v>
       </c>
@@ -1529,8 +1698,11 @@
       <c r="E56">
         <v>770</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
@@ -1546,8 +1718,11 @@
       <c r="E57">
         <v>477</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
@@ -1563,8 +1738,11 @@
       <c r="E58">
         <v>844</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>27</v>
       </c>
@@ -1580,8 +1758,11 @@
       <c r="E59">
         <v>835</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>27</v>
       </c>
@@ -1597,8 +1778,11 @@
       <c r="E60">
         <v>541</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>27</v>
       </c>
@@ -1614,8 +1798,11 @@
       <c r="E61">
         <v>925</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>28</v>
       </c>
@@ -1631,8 +1818,11 @@
       <c r="E62">
         <v>871</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>28</v>
       </c>
@@ -1648,8 +1838,11 @@
       <c r="E63">
         <v>540</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>28</v>
       </c>
@@ -1665,8 +1858,11 @@
       <c r="E64">
         <v>941</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>29</v>
       </c>
@@ -1682,8 +1878,11 @@
       <c r="E65">
         <v>877</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>29</v>
       </c>
@@ -1699,8 +1898,11 @@
       <c r="E66">
         <v>551</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>29</v>
       </c>
@@ -1716,8 +1918,11 @@
       <c r="E67">
         <v>958</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>30</v>
       </c>
@@ -1733,8 +1938,11 @@
       <c r="E68">
         <v>876</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>30</v>
       </c>
@@ -1750,8 +1958,11 @@
       <c r="E69">
         <v>557</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>30</v>
       </c>
@@ -1767,8 +1978,11 @@
       <c r="E70">
         <v>949</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>31</v>
       </c>
@@ -1784,8 +1998,11 @@
       <c r="E71">
         <v>877</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>31</v>
       </c>
@@ -1801,8 +2018,11 @@
       <c r="E72">
         <v>548</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>31</v>
       </c>
@@ -1818,8 +2038,11 @@
       <c r="E73">
         <v>952</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>32</v>
       </c>
@@ -1835,8 +2058,11 @@
       <c r="E74">
         <v>585</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>32</v>
       </c>
@@ -1852,8 +2078,11 @@
       <c r="E75">
         <v>331</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>32</v>
       </c>
@@ -1869,8 +2098,11 @@
       <c r="E76">
         <v>696</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>33</v>
       </c>
@@ -1886,8 +2118,11 @@
       <c r="E77">
         <v>667</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>33</v>
       </c>
@@ -1903,8 +2138,11 @@
       <c r="E78">
         <v>389</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>33</v>
       </c>
@@ -1920,8 +2158,11 @@
       <c r="E79">
         <v>775</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>34</v>
       </c>
@@ -1937,8 +2178,11 @@
       <c r="E80">
         <v>734</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>34</v>
       </c>
@@ -1954,8 +2198,11 @@
       <c r="E81">
         <v>444</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>34</v>
       </c>
@@ -1971,8 +2218,11 @@
       <c r="E82">
         <v>895</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>35</v>
       </c>
@@ -1988,8 +2238,11 @@
       <c r="E83">
         <v>771</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>35</v>
       </c>
@@ -2005,8 +2258,11 @@
       <c r="E84">
         <v>459</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>35</v>
       </c>
@@ -2022,8 +2278,11 @@
       <c r="E85">
         <v>877</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>36</v>
       </c>
@@ -2039,8 +2298,11 @@
       <c r="E86">
         <v>765</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>36</v>
       </c>
@@ -2056,8 +2318,11 @@
       <c r="E87">
         <v>468</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>36</v>
       </c>
@@ -2073,8 +2338,11 @@
       <c r="E88">
         <v>877</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>37</v>
       </c>
@@ -2090,8 +2358,11 @@
       <c r="E89">
         <v>746</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>37</v>
       </c>
@@ -2107,8 +2378,11 @@
       <c r="E90">
         <v>447</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>37</v>
       </c>
@@ -2124,8 +2398,11 @@
       <c r="E91">
         <v>858</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>38</v>
       </c>
@@ -2141,8 +2418,11 @@
       <c r="E92">
         <v>752</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>38</v>
       </c>
@@ -2158,8 +2438,11 @@
       <c r="E93">
         <v>430</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>38</v>
       </c>
@@ -2175,8 +2458,11 @@
       <c r="E94">
         <v>833</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>39</v>
       </c>
@@ -2192,8 +2478,11 @@
       <c r="E95">
         <v>779</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>39</v>
       </c>
@@ -2209,8 +2498,11 @@
       <c r="E96">
         <v>487</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>39</v>
       </c>
@@ -2226,8 +2518,11 @@
       <c r="E97">
         <v>888</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>40</v>
       </c>
@@ -2243,8 +2538,11 @@
       <c r="E98">
         <v>796</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>40</v>
       </c>
@@ -2260,8 +2558,11 @@
       <c r="E99">
         <v>490</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>40</v>
       </c>
@@ -2277,8 +2578,11 @@
       <c r="E100">
         <v>910</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>41</v>
       </c>
@@ -2294,8 +2598,11 @@
       <c r="E101">
         <v>828</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>41</v>
       </c>
@@ -2311,8 +2618,11 @@
       <c r="E102">
         <v>498</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>41</v>
       </c>
@@ -2328,8 +2638,11 @@
       <c r="E103">
         <v>918</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>42</v>
       </c>
@@ -2345,8 +2658,11 @@
       <c r="E104">
         <v>816</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>42</v>
       </c>
@@ -2362,8 +2678,11 @@
       <c r="E105">
         <v>501</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>42</v>
       </c>
@@ -2379,8 +2698,11 @@
       <c r="E106">
         <v>928</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>43</v>
       </c>
@@ -2396,8 +2718,11 @@
       <c r="E107">
         <v>845</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>43</v>
       </c>
@@ -2413,8 +2738,11 @@
       <c r="E108">
         <v>495</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>43</v>
       </c>
@@ -2430,8 +2758,11 @@
       <c r="E109">
         <v>959</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>44</v>
       </c>
@@ -2447,8 +2778,11 @@
       <c r="E110">
         <v>512</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>44</v>
       </c>
@@ -2464,8 +2798,11 @@
       <c r="E111">
         <v>275</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>44</v>
       </c>
@@ -2481,8 +2818,11 @@
       <c r="E112">
         <v>639</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>45</v>
       </c>
@@ -2498,8 +2838,11 @@
       <c r="E113">
         <v>526</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>45</v>
       </c>
@@ -2515,8 +2858,11 @@
       <c r="E114">
         <v>286</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>45</v>
       </c>
@@ -2532,8 +2878,11 @@
       <c r="E115">
         <v>658</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>46</v>
       </c>
@@ -2549,8 +2898,11 @@
       <c r="E116">
         <v>531</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>46</v>
       </c>
@@ -2566,8 +2918,11 @@
       <c r="E117">
         <v>286</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>46</v>
       </c>
@@ -2583,8 +2938,11 @@
       <c r="E118">
         <v>664</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>47</v>
       </c>
@@ -2600,8 +2958,11 @@
       <c r="E119">
         <v>449</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>47</v>
       </c>
@@ -2617,8 +2978,11 @@
       <c r="E120">
         <v>250</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>47</v>
       </c>
@@ -2634,8 +2998,11 @@
       <c r="E121">
         <v>566</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>48</v>
       </c>
@@ -2651,8 +3018,11 @@
       <c r="E122">
         <v>476</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>48</v>
       </c>
@@ -2668,8 +3038,11 @@
       <c r="E123">
         <v>266</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>48</v>
       </c>
@@ -2685,8 +3058,11 @@
       <c r="E124">
         <v>592</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>49</v>
       </c>
@@ -2702,8 +3078,11 @@
       <c r="E125">
         <v>497</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>49</v>
       </c>
@@ -2719,8 +3098,11 @@
       <c r="E126">
         <v>277</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>49</v>
       </c>
@@ -2736,8 +3118,11 @@
       <c r="E127">
         <v>617</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>50</v>
       </c>
@@ -2753,8 +3138,11 @@
       <c r="E128">
         <v>517</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>50</v>
       </c>
@@ -2770,8 +3158,11 @@
       <c r="E129">
         <v>288</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>50</v>
       </c>
@@ -2787,8 +3178,11 @@
       <c r="E130">
         <v>635</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>51</v>
       </c>
@@ -2804,8 +3198,11 @@
       <c r="E131">
         <v>553</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>51</v>
       </c>
@@ -2821,8 +3218,11 @@
       <c r="E132">
         <v>322</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F132">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>51</v>
       </c>
@@ -2838,8 +3238,11 @@
       <c r="E133">
         <v>680</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>52</v>
       </c>
@@ -2855,8 +3258,11 @@
       <c r="E134">
         <v>600</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>52</v>
       </c>
@@ -2872,8 +3278,11 @@
       <c r="E135">
         <v>338</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>52</v>
       </c>
@@ -2889,8 +3298,11 @@
       <c r="E136">
         <v>742</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>53</v>
       </c>
@@ -2906,8 +3318,11 @@
       <c r="E137">
         <v>652</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>53</v>
       </c>
@@ -2923,8 +3338,11 @@
       <c r="E138">
         <v>365</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>53</v>
       </c>
@@ -2940,8 +3358,11 @@
       <c r="E139">
         <v>764</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>54</v>
       </c>
@@ -2957,8 +3378,11 @@
       <c r="E140">
         <v>679</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>54</v>
       </c>
@@ -2974,8 +3398,11 @@
       <c r="E141">
         <v>382</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>54</v>
       </c>
@@ -2991,8 +3418,11 @@
       <c r="E142">
         <v>792</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>55</v>
       </c>
@@ -3008,8 +3438,11 @@
       <c r="E143">
         <v>712</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>55</v>
       </c>
@@ -3025,8 +3458,11 @@
       <c r="E144">
         <v>398</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>55</v>
       </c>
@@ -3042,8 +3478,11 @@
       <c r="E145">
         <v>850</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>56</v>
       </c>
@@ -3059,8 +3498,11 @@
       <c r="E146">
         <v>1001</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>56</v>
       </c>
@@ -3076,8 +3518,11 @@
       <c r="E147">
         <v>598</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>56</v>
       </c>
@@ -3093,8 +3538,11 @@
       <c r="E148">
         <v>1099</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>57</v>
       </c>
@@ -3110,8 +3558,11 @@
       <c r="E149">
         <v>1107</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>57</v>
       </c>
@@ -3127,8 +3578,11 @@
       <c r="E150">
         <v>678</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>57</v>
       </c>
@@ -3144,8 +3598,11 @@
       <c r="E151">
         <v>1209</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>58</v>
       </c>
@@ -3161,8 +3618,11 @@
       <c r="E152">
         <v>1114</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>58</v>
       </c>
@@ -3178,8 +3638,11 @@
       <c r="E153">
         <v>695</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>58</v>
       </c>
@@ -3195,8 +3658,11 @@
       <c r="E154">
         <v>1234</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F154">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>59</v>
       </c>
@@ -3212,8 +3678,11 @@
       <c r="E155">
         <v>230</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F155">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>59</v>
       </c>
@@ -3229,8 +3698,11 @@
       <c r="E156">
         <v>136</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F156">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>59</v>
       </c>
@@ -3246,8 +3718,11 @@
       <c r="E157">
         <v>312</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F157">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>60</v>
       </c>
@@ -3263,8 +3738,11 @@
       <c r="E158">
         <v>241</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F158">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>60</v>
       </c>
@@ -3280,8 +3758,11 @@
       <c r="E159">
         <v>145</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F159">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>60</v>
       </c>
@@ -3297,8 +3778,11 @@
       <c r="E160">
         <v>333</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F160">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>61</v>
       </c>
@@ -3314,8 +3798,11 @@
       <c r="E161">
         <v>319</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F161">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>61</v>
       </c>
@@ -3331,8 +3818,11 @@
       <c r="E162">
         <v>175</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>61</v>
       </c>
@@ -3348,8 +3838,11 @@
       <c r="E163">
         <v>425</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F163">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>62</v>
       </c>
@@ -3365,8 +3858,11 @@
       <c r="E164">
         <v>384</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F164">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>62</v>
       </c>
@@ -3382,8 +3878,11 @@
       <c r="E165">
         <v>208</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F165">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>62</v>
       </c>
@@ -3399,8 +3898,11 @@
       <c r="E166">
         <v>510</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F166">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>63</v>
       </c>
@@ -3416,8 +3918,11 @@
       <c r="E167">
         <v>438</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F167">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>63</v>
       </c>
@@ -3433,8 +3938,11 @@
       <c r="E168">
         <v>229</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F168">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>63</v>
       </c>
@@ -3450,8 +3958,11 @@
       <c r="E169">
         <v>565</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>64</v>
       </c>
@@ -3467,8 +3978,11 @@
       <c r="E170">
         <v>473</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F170">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>64</v>
       </c>
@@ -3484,8 +3998,11 @@
       <c r="E171">
         <v>255</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F171">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>64</v>
       </c>
@@ -3501,8 +4018,11 @@
       <c r="E172">
         <v>595</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F172">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>65</v>
       </c>
@@ -3518,8 +4038,11 @@
       <c r="E173">
         <v>514</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F173">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>65</v>
       </c>
@@ -3535,8 +4058,11 @@
       <c r="E174">
         <v>275</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F174">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>65</v>
       </c>
@@ -3552,8 +4078,11 @@
       <c r="E175">
         <v>648</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>66</v>
       </c>
@@ -3569,8 +4098,11 @@
       <c r="E176">
         <v>545</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>66</v>
       </c>
@@ -3586,8 +4118,11 @@
       <c r="E177">
         <v>286</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F177">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>66</v>
       </c>
@@ -3603,8 +4138,11 @@
       <c r="E178">
         <v>681</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>67</v>
       </c>
@@ -3620,8 +4158,11 @@
       <c r="E179">
         <v>557</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>67</v>
       </c>
@@ -3637,8 +4178,11 @@
       <c r="E180">
         <v>288</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F180">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>67</v>
       </c>
@@ -3653,6 +4197,9 @@
       </c>
       <c r="E181">
         <v>719</v>
+      </c>
+      <c r="F181">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>